<commit_message>
end of day 7/03 - aggregated DA constraint task
</commit_message>
<xml_diff>
--- a/Network Topology/CRR Bus and Branches.xlsx
+++ b/Network Topology/CRR Bus and Branches.xlsx
@@ -443,350 +443,350 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GATES  9:11572,11579,GATES  9,GATES 16/11572,30060,GATES  9,MIDWAY1</t>
+          <t>GATES  9:11572,30060,GATES  9,MIDWAY10/11572,11579,GATES  9,GATES 16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">GATES 10:11573,11578,GATES 10,GATES 15/11573,30050,GATES 10,LOSBNS </t>
+          <t>GATES 10:11573,30050,GATES 10,LOSBNS 4/11573,11578,GATES 10,GATES 15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GATES 11:11574,11577,GATES 11,GATES 14/30056,11574,GATES  7,GATES 1</t>
+          <t>GATES 11:30056,11574,GATES  7,GATES 11/11574,11577,GATES 11,GATES 14</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">GATES 12:11575,11576,GATES 12,GATES 13/11575,30050,GATES 12,LOSBNS </t>
+          <t>GATES 12:11575,11576,GATES 12,GATES 13/11575,30050,GATES 12,LOSBNS 4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GATES 13:11575,11576,GATES 12,GATES 13/30055,11576,GATES  8,GATES 1</t>
+          <t>GATES 13:30055,11576,GATES  8,GATES 13/11575,11576,GATES 12,GATES 13</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GATES 14:11577,30060,GATES 14,MIDWAY10/11574,11577,GATES 11,GATES 1</t>
+          <t>GATES 14:11574,11577,GATES 11,GATES 14/11577,30060,GATES 14,MIDWAY10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GATES 15:11573,11578,GATES 10,GATES 15/30056,11578,GATES  7,GATES 1</t>
+          <t>GATES 15:30056,11578,GATES  7,GATES 15/11573,11578,GATES 10,GATES 15</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GATES 16:11572,11579,GATES  9,GATES 16/30055,11579,GATES  8,GATES 1</t>
+          <t>GATES 16:30055,11579,GATES  8,GATES 16/11572,11579,GATES  9,GATES 16</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">GATES  </t>
+          <t>GATES  4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">METCLF </t>
+          <t>METCLF 4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">METCLF </t>
+          <t>METCLF 5</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MIDWAY11:30060,11747,MIDWAY10,MIDWAY1</t>
+          <t>MIDWAY11:30060,11747,MIDWAY10,MIDWAY11</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MIDWAY12:30060,11748,MIDWAY10,MIDWAY1</t>
+          <t>MIDWAY12:30060,11748,MIDWAY10,MIDWAY12</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MIDWAY13:30060,11749,MIDWAY10,MIDWAY1</t>
+          <t>MIDWAY13:30060,11749,MIDWAY10,MIDWAY13</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">MIDWAY </t>
+          <t>MIDWAY 1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNDMTN 5:11878,11949,RNDMTN 5,TBLMTN11/30005,11878,RNDMTN 4,RNDMTN </t>
+          <t>RNDMTN 5:11878,11949,RNDMTN 5,TBLMTN11/30005,11878,RNDMTN 4,RNDMTN 5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNDMTN 6:11879,11882,RNDMTN 6,RNDMTN 9/30005,11879,RNDMTN 4,RNDMTN </t>
+          <t>RNDMTN 6:11879,11882,RNDMTN 6,RNDMTN 9/30005,11879,RNDMTN 4,RNDMTN 6</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNDMTN 7:11880,11948,RNDMTN 7,TBLMTN10/30005,11880,RNDMTN 4,RNDMTN </t>
+          <t>RNDMTN 7:11880,11948,RNDMTN 7,TBLMTN10/30005,11880,RNDMTN 4,RNDMTN 7</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RNDMTN 8:30005,11881,RNDMTN 4,RNDMTN 8/11881,11883,RNDMTN 8,RNDMTN1</t>
+          <t>RNDMTN 8:30005,11881,RNDMTN 4,RNDMTN 8/11881,11883,RNDMTN 8,RNDMTN10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNDMTN 9:11879,11882,RNDMTN 6,RNDMTN </t>
+          <t>RNDMTN 9:11879,11882,RNDMTN 6,RNDMTN 9</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RNDMTN10:30010,11883,INDNSP 1,RNDMTN10/11881,11883,RNDMTN 8,RNDMTN1</t>
+          <t>RNDMTN10:30010,11883,INDNSP 1,RNDMTN10/11881,11883,RNDMTN 8,RNDMTN10</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TBLMTN 7:11945,11952,TBLMTN 7,TBLMTN12/11945,11965,TBLMTN 7,TESLA 1</t>
+          <t>TBLMTN 7:11945,11965,TBLMTN 7,TESLA 12/11945,11952,TBLMTN 7,TBLMTN12</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">TBLMTN 8:11946,11947,TBLMTN 8,TBLMTN 9/30015,11946,TBLMTN 6,TBLMTN </t>
+          <t>TBLMTN 8:30015,11946,TBLMTN 6,TBLMTN 8/11946,11947,TBLMTN 8,TBLMTN 9</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">TBLMTN 9:11946,11947,TBLMTN 8,TBLMTN 9/11947,11990,TBLMTN 9,VACADX </t>
+          <t>TBLMTN 9:11947,11990,TBLMTN 9,VACADX 9/11946,11947,TBLMTN 8,TBLMTN 9</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TBLMTN10:11880,11948,RNDMTN 7,TBLMTN10/30015,11948,TBLMTN 6,TBLMTN1</t>
+          <t>TBLMTN10:11880,11948,RNDMTN 7,TBLMTN10/30015,11948,TBLMTN 6,TBLMTN10</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TBLMTN11:11878,11949,RNDMTN 5,TBLMTN11/30015,11949,TBLMTN 6,TBLMTN1</t>
+          <t>TBLMTN11:11878,11949,RNDMTN 5,TBLMTN11/30015,11949,TBLMTN 6,TBLMTN11</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">TBLMTN </t>
+          <t>TBLMTN 2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve">TBLMTN </t>
+          <t>TBLMTN 3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TBLMTN12:11945,11952,TBLMTN 7,TBLMTN12/30015,11952,TBLMTN 6,TBLMTN1</t>
+          <t>TBLMTN12:30015,11952,TBLMTN 6,TBLMTN12/11945,11952,TBLMTN 7,TBLMTN12</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TESLA 12:11965,11966,TESLA 12,TESLA 13/11945,11965,TBLMTN 7,TESLA 1</t>
+          <t>TESLA 12:11945,11965,TBLMTN 7,TESLA 12/11965,11966,TESLA 12,TESLA 13</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TESLA 13:11965,11966,TESLA 12,TESLA 13/30040,11966,TESLA 10,TESLA 1</t>
+          <t>TESLA 13:30040,11966,TESLA 10,TESLA 13/11965,11966,TESLA 12,TESLA 13</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">VACADX 9:11990,11993,VACADX 9,VACADX12/11947,11990,TBLMTN 9,VACADX </t>
+          <t>VACADX 9:11947,11990,TBLMTN 9,VACADX 9/11990,11993,VACADX 9,VACADX12</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>VACADX10:11991,11992,VACADX10,VACADX11/30040,11991,TESLA 10,VACADX1</t>
+          <t>VACADX10:30040,11991,TESLA 10,VACADX10/11991,11992,VACADX10,VACADX11</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>VACADX11:11991,11992,VACADX10,VACADX11/30030,11992,VACADX 8,VACADX1</t>
+          <t>VACADX11:30030,11992,VACADX 8,VACADX11/11991,11992,VACADX10,VACADX11</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>VACADX12:30030,11993,VACADX 8,VACADX12/11990,11993,VACADX 9,VACADX1</t>
+          <t>VACADX12:11990,11993,VACADX 9,VACADX12/30030,11993,VACADX 8,VACADX12</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNDMTN 4:30005,11878,RNDMTN 4,RNDMTN 5/30005,11881,RNDMTN 4,RNDMTN 8/30005,11879,RNDMTN 4,RNDMTN 6/30005,11880,RNDMTN 4,RNDMTN </t>
+          <t>RNDMTN 4:30005,11881,RNDMTN 4,RNDMTN 8/30005,11879,RNDMTN 4,RNDMTN 6/30005,11880,RNDMTN 4,RNDMTN 7/30005,11878,RNDMTN 4,RNDMTN 5</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>INDNSP 1:30010,11883,INDNSP 1,RNDMTN1</t>
+          <t>INDNSP 1:30010,11883,INDNSP 1,RNDMTN10</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">TBLMTN 6:30015,11949,TBLMTN 6,TBLMTN11/30015,11952,TBLMTN 6,TBLMTN12/30015,11948,TBLMTN 6,TBLMTN10/30015,11946,TBLMTN 6,TBLMTN </t>
+          <t>TBLMTN 6:30015,11952,TBLMTN 6,TBLMTN12/30015,11948,TBLMTN 6,TBLMTN10/30015,11946,TBLMTN 6,TBLMTN 8/30015,11949,TBLMTN 6,TBLMTN11</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>VACADX 8:30030,11992,VACADX 8,VACADX11/30030,11993,VACADX 8,VACADX1</t>
+          <t>VACADX 8:30030,11992,VACADX 8,VACADX11/30030,11993,VACADX 8,VACADX12</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TESLA 10:30040,11991,TESLA 10,VACADX10/30042,30040,METCLF 5,TESLA 10/30050,30040,LOSBNS 4,TESLA 10/30040,11966,TESLA 10,TESLA 13/30040,99006,TESLA 10,TESLA 1</t>
+          <t>TESLA 10:30040,11991,TESLA 10,VACADX10/30050,30040,LOSBNS 4,TESLA 10/30042,30040,METCLF 5,TESLA 10/30040,99006,TESLA 10,TESLA 11/30040,11966,TESLA 10,TESLA 13</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>METCLF 5:30042,30040,METCLF 5,TESLA 10/30042,30045,METCLF 5,MOSSLD1</t>
+          <t>METCLF 5:30042,30040,METCLF 5,TESLA 10/30042,30045,METCLF 5,MOSSLD13</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MOSSLD13:30050,30045,LOSBNS 4,MOSSLD13/30045,30046,MOSSLD13,VISTRA 4/30042,30045,METCLF 5,MOSSLD1</t>
+          <t>MOSSLD13:30042,30045,METCLF 5,MOSSLD13/30045,30046,MOSSLD13,VISTRA 4/30050,30045,LOSBNS 4,MOSSLD13</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">VISTRA 4:30045,30046,MOSSLD13,VISTRA </t>
+          <t>VISTRA 4:30045,30046,MOSSLD13,VISTRA 4</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">LOSBNS 4:30050,30045,LOSBNS 4,MOSSLD13/11573,30050,GATES 10,LOSBNS 4/11575,30050,GATES 12,LOSBNS 4/30050,30040,LOSBNS 4,TESLA 10/30050,99005,LOSBNS 4,LOSBNS 5/30055,30050,GATES  8,LOSBNS </t>
+          <t>LOSBNS 4:11573,30050,GATES 10,LOSBNS 4/11575,30050,GATES 12,LOSBNS 4/30050,30040,LOSBNS 4,TESLA 10/30055,30050,GATES  8,LOSBNS 4/30050,99005,LOSBNS 4,LOSBNS 5/30050,30045,LOSBNS 4,MOSSLD13</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">GATES  8:30055,30050,GATES  8,LOSBNS 4/30055,11576,GATES  8,GATES 13/30055,11579,GATES  8,GATES 16/30057,30055,DIABLO 4,GATES  </t>
+          <t>GATES  8:30057,30055,DIABLO 4,GATES  8/30055,30050,GATES  8,LOSBNS 4/30055,11576,GATES  8,GATES 13/30055,11579,GATES  8,GATES 16</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GATES  7:30056,11574,GATES  7,GATES 11/30056,11578,GATES  7,GATES 1</t>
+          <t>GATES  7:30056,11578,GATES  7,GATES 15/30056,11574,GATES  7,GATES 11</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t xml:space="preserve">DIABLO 4:30057,30060,DIABLO 4,MIDWAY10/30057,30060,DIABLO 4,MIDWAY10/30057,30055,DIABLO 4,GATES  </t>
+          <t>DIABLO 4:30057,30060,DIABLO 4,MIDWAY10/30057,30055,DIABLO 4,GATES  8/30057,30060,DIABLO 4,MIDWAY10</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MIDWAY10:30057,30060,DIABLO 4,MIDWAY10/30060,11747,MIDWAY10,MIDWAY11/11577,30060,GATES 14,MIDWAY10/30060,11749,MIDWAY10,MIDWAY13/30060,11748,MIDWAY10,MIDWAY12/11572,30060,GATES  9,MIDWAY10/30057,30060,DIABLO 4,MIDWAY1</t>
+          <t>MIDWAY10:30060,11749,MIDWAY10,MIDWAY13/11577,30060,GATES 14,MIDWAY10/30060,11748,MIDWAY10,MIDWAY12/11572,30060,GATES  9,MIDWAY10/30057,30060,DIABLO 4,MIDWAY10/30060,11747,MIDWAY10,MIDWAY11/30057,30060,DIABLO 4,MIDWAY10</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">LOSBNS 5:30050,99005,LOSBNS 4,LOSBNS </t>
+          <t>LOSBNS 5:30050,99005,LOSBNS 4,LOSBNS 5</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TESLA 11:30040,99006,TESLA 10,TESLA 1</t>
+          <t>TESLA 11:30040,99006,TESLA 10,TESLA 11</t>
         </is>
       </c>
     </row>

</xml_diff>